<commit_message>
correction bug(lors ajout nounours sur meme nounous dont chiffre modifié dans panier(et string au lieu number->ajout string au lieu nombre..) test: edit
</commit_message>
<xml_diff>
--- a/tests/plan-de-tests.xlsx
+++ b/tests/plan-de-tests.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
   <si>
     <t xml:space="preserve">Fichier JS</t>
   </si>
@@ -40,27 +40,6 @@
     <t xml:space="preserve">Problème possible</t>
   </si>
   <si>
-    <t xml:space="preserve">à effacer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 à 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">userInputChecker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La fonction doit retourner 1 si le mot passé en paramètre est un mot (pas de chiffre, caractères accentués, symboles ...), et retourner 0 si ce n'en est pas un</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Appeller la fonction avec différentes valeurs de tests (valeurs limites, valeur vide...), et on observe la valeur retournée, avec un console.log par exemple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La valeur retournée pourrait être érronée (0 au lieu de 1;  et 1 au lieu de 0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXEMPLE </t>
-  </si>
-  <si>
     <t xml:space="preserve">script.js</t>
   </si>
   <si>
@@ -76,7 +55,7 @@
     <t xml:space="preserve">tester avec wrong-url, avec pas de connection back-end(stop server local pour le simuler)</t>
   </si>
   <si>
-    <t xml:space="preserve">erreur non captée</t>
+    <t xml:space="preserve">erreur non captée (console,log)</t>
   </si>
   <si>
     <t xml:space="preserve">3-11</t>
@@ -408,7 +387,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -439,22 +418,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFBF0041"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="0"/>
@@ -466,7 +429,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -481,12 +444,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEEEEEE"/>
-        <bgColor rgb="FFDEE6EF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFDDE8CB"/>
         <bgColor rgb="FFDEE6EF"/>
       </patternFill>
@@ -494,7 +451,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDEE6EF"/>
-        <bgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFDDE8CB"/>
       </patternFill>
     </fill>
     <fill>
@@ -510,19 +467,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -628,7 +578,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="54">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -645,23 +595,63 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -669,15 +659,35 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -689,27 +699,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -717,23 +715,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -741,15 +731,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -757,15 +747,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -773,31 +763,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -805,55 +783,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -869,7 +807,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFEEEEEE"/>
+      <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -880,7 +818,7 @@
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FFBF0041"/>
+      <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFF7D1D5"/>
       <rgbColor rgb="FF808080"/>
@@ -934,12 +872,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -998,626 +936,608 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="6" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+      <c r="C5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="D5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="E5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="F5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="11" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+    </row>
+    <row r="7" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="B7" s="18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13"/>
-      <c r="B6" s="14" t="s">
+      <c r="C7" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="D7" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="E7" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="F7" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="17" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="22"/>
+      <c r="B8" s="23" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-    </row>
-    <row r="8" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20" t="s">
+      <c r="C8" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="D8" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="E8" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="F8" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="23" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="27"/>
+      <c r="B9" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="C9" s="29" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="25"/>
-      <c r="B9" s="26" t="s">
+      <c r="D9" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="E9" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="F9" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="28" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+    </row>
+    <row r="11" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="B11" s="33" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="30"/>
-      <c r="B10" s="31" t="s">
+      <c r="C11" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="D11" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="E11" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="33" t="s">
+      <c r="F11" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="34" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="36"/>
+      <c r="B12" s="37" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-    </row>
-    <row r="12" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="35" t="s">
+      <c r="C12" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="D12" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="E12" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="F12" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="37" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="36"/>
+      <c r="B13" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="38" t="s">
+      <c r="C13" s="37" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="39"/>
-      <c r="B13" s="40" t="s">
+      <c r="D13" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="E13" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="41" t="s">
+      <c r="F13" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="41" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="36"/>
+      <c r="B14" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="42" t="s">
+      <c r="C14" s="37" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="39"/>
-      <c r="B14" s="40" t="s">
+      <c r="D14" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="E14" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="41" t="s">
+      <c r="F14" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="41" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="36"/>
+      <c r="B15" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="42" t="s">
+      <c r="C15" s="37" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="39"/>
-      <c r="B15" s="40" t="s">
+      <c r="D15" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="E15" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="41" t="s">
+      <c r="F15" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="41" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="36"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="42" t="s">
+      <c r="F16" s="39" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="39"/>
-      <c r="B16" s="40" t="s">
+    <row r="17" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="36"/>
+      <c r="B17" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="40" t="s">
+      <c r="C17" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="41" t="s">
+      <c r="D17" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="41" t="s">
+      <c r="E17" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="F16" s="42" t="s">
+      <c r="F17" s="39" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="39"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41" t="s">
+      <c r="G17" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="42" t="s">
+      <c r="H17" s="0" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="39"/>
-      <c r="B18" s="40" t="s">
+      <c r="A18" s="36"/>
+      <c r="B18" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="41" t="s">
+      <c r="D18" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="41" t="s">
+      <c r="E18" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="F18" s="42" t="s">
+      <c r="F18" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="G18" s="0" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="36"/>
+      <c r="B19" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="H18" s="0" t="s">
+      <c r="C19" s="37" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="39"/>
-      <c r="B19" s="40" t="s">
+      <c r="D19" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="40" t="s">
+      <c r="E19" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="41" t="s">
+      <c r="F19" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="E19" s="41" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="36"/>
+      <c r="B20" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="F19" s="42" t="s">
+      <c r="C20" s="37" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="39"/>
-      <c r="B20" s="40" t="s">
+      <c r="D20" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="40" t="s">
+      <c r="E20" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="D20" s="41" t="s">
+      <c r="F20" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="E20" s="41" t="s">
+    </row>
+    <row r="21" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="36"/>
+      <c r="B21" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="F20" s="42" t="s">
+      <c r="C21" s="37" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="39"/>
-      <c r="B21" s="40" t="s">
+      <c r="D21" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="C21" s="40" t="s">
+      <c r="E21" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="41" t="s">
+      <c r="F21" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="E21" s="41" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="36"/>
+      <c r="B22" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="F21" s="42" t="s">
+      <c r="C22" s="37" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="39"/>
-      <c r="B22" s="40" t="s">
+      <c r="D22" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="E22" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="D22" s="41" t="s">
+      <c r="F22" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="E22" s="41" t="s">
+    </row>
+    <row r="23" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="36"/>
+      <c r="B23" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="F22" s="42" t="s">
+      <c r="C23" s="37" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="39"/>
-      <c r="B23" s="40" t="s">
+      <c r="D23" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="C23" s="40" t="s">
+      <c r="E23" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="D23" s="41" t="s">
+      <c r="F23" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="E23" s="41" t="s">
+    </row>
+    <row r="24" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="40"/>
+      <c r="B24" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="F23" s="42" t="s">
+      <c r="C24" s="41" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="39"/>
-      <c r="B24" s="40" t="s">
+      <c r="D24" s="42" t="s">
         <v>100</v>
       </c>
-      <c r="C24" s="40" t="s">
+      <c r="E24" s="42" t="s">
         <v>101</v>
       </c>
-      <c r="D24" s="41" t="s">
+      <c r="F24" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="E24" s="41" t="s">
+    </row>
+    <row r="25" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+    </row>
+    <row r="26" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="F24" s="42" t="s">
+      <c r="B26" s="45" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="43"/>
-      <c r="B25" s="44" t="s">
+      <c r="C26" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="C25" s="44" t="s">
+      <c r="D26" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="D25" s="45" t="s">
+      <c r="E26" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="E25" s="45" t="s">
+      <c r="F26" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="F25" s="46" t="s">
+    </row>
+    <row r="27" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="49"/>
+      <c r="B27" s="50" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-    </row>
-    <row r="27" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="47" t="s">
+      <c r="C27" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="B27" s="48" t="s">
+      <c r="D27" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="C27" s="49" t="s">
+      <c r="E27" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="D27" s="50" t="s">
+      <c r="F27" s="53" t="s">
         <v>113</v>
       </c>
-      <c r="E27" s="50" t="s">
-        <v>114</v>
-      </c>
-      <c r="F27" s="51" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="28" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="52"/>
-      <c r="B28" s="53" t="s">
-        <v>116</v>
-      </c>
-      <c r="C28" s="54" t="s">
-        <v>117</v>
-      </c>
-      <c r="D28" s="55" t="s">
-        <v>118</v>
-      </c>
-      <c r="E28" s="55" t="s">
-        <v>119</v>
-      </c>
-      <c r="F28" s="56" t="s">
-        <v>120</v>
-      </c>
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
     </row>
     <row r="29" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="18"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
     </row>
     <row r="30" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="18"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
     </row>
     <row r="31" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="18"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
     </row>
     <row r="32" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
     </row>
     <row r="33" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
     </row>
     <row r="34" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
     </row>
     <row r="35" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="18"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
+      <c r="A35" s="15"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
     </row>
     <row r="36" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="18"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
+      <c r="A36" s="15"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
     </row>
     <row r="37" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="18"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
     </row>
     <row r="38" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="18"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
     </row>
     <row r="39" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="18"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
+      <c r="A39" s="15"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
     </row>
     <row r="40" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="18"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
     </row>
     <row r="41" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="18"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
+      <c r="A41" s="15"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
     </row>
     <row r="42" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="18"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
+      <c r="A42" s="15"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
     </row>
     <row r="43" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="18"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
+      <c r="A43" s="15"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
     </row>
     <row r="44" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="18"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="19"/>
+      <c r="A44" s="15"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
     </row>
     <row r="45" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="18"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-    </row>
-    <row r="46" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="18"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
+      <c r="A45" s="15"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+    </row>
+    <row r="46" customFormat="false" ht="61.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="15"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
     </row>
     <row r="47" customFormat="false" ht="61.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="18"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="19"/>
+      <c r="A47" s="15"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
     </row>
     <row r="48" customFormat="false" ht="61.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="18"/>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19"/>
+      <c r="A48" s="15"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
     </row>
     <row r="49" customFormat="false" ht="61.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="18"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
+      <c r="A49" s="15"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
     </row>
     <row r="50" customFormat="false" ht="61.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="18"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-    </row>
-    <row r="51" customFormat="false" ht="61.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="18"/>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
+      <c r="A50" s="15"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+    </row>
+    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D52" s="3"/>
@@ -6359,11 +6279,7 @@
       <c r="E999" s="3"/>
       <c r="F999" s="3"/>
     </row>
-    <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1000" s="3"/>
-      <c r="E1000" s="3"/>
-      <c r="F1000" s="3"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>